<commit_message>
Added a MS-1 test to the FPGA Bitstream spreadsheet
</commit_message>
<xml_diff>
--- a/results/fpgaBitstream/SpatterFPGABitstreamBenchmarks.xlsx
+++ b/results/fpgaBitstream/SpatterFPGABitstreamBenchmarks.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jowu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09579D2-5C8F-B04D-A5FE-BB3FF270BC4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732DA2A-B3D7-9B46-8ED7-50D7F4416F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="580" windowWidth="28040" windowHeight="16880" xr2:uid="{3A13CA78-B1F6-EF46-A702-6420C2607B68}"/>
+    <workbookView xWindow="8020" yWindow="460" windowWidth="28040" windowHeight="16880" xr2:uid="{3A13CA78-B1F6-EF46-A702-6420C2607B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Delta</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Conditions (10 runs for each delta)</t>
+  </si>
+  <si>
+    <t>Length = 512, Pattern = MS1:8:4:8, Runs = 50</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB82E855-A4B2-7043-BC13-3BE390FD896D}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:O2" si="0">J2 + 1</f>
+        <f t="shared" ref="K2:N2" si="0">J2 + 1</f>
         <v>9</v>
       </c>
       <c r="L2">
@@ -1408,7 +1411,7 @@
         <v>6197.26</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>6598.38</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>6757.16</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>6197.26</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1570,6 +1573,601 @@
       <c r="K36">
         <f t="shared" si="8"/>
         <v>171.77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>4626.29</v>
+      </c>
+      <c r="D38">
+        <v>4848.7700000000004</v>
+      </c>
+      <c r="E38">
+        <v>4828.05</v>
+      </c>
+      <c r="F38">
+        <v>4794.8500000000004</v>
+      </c>
+      <c r="G38">
+        <v>4868.22</v>
+      </c>
+      <c r="H38">
+        <v>4815.99</v>
+      </c>
+      <c r="I38">
+        <v>4878.37</v>
+      </c>
+      <c r="J38">
+        <v>4545.43</v>
+      </c>
+      <c r="K38">
+        <v>4892.21</v>
+      </c>
+      <c r="L38">
+        <v>4964.8500000000004</v>
+      </c>
+      <c r="M38">
+        <v>4959.59</v>
+      </c>
+      <c r="N38">
+        <v>4926.04</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>4537.88</v>
+      </c>
+      <c r="D39">
+        <v>4537.25</v>
+      </c>
+      <c r="E39">
+        <v>4541.0200000000004</v>
+      </c>
+      <c r="F39">
+        <v>4575.8999999999996</v>
+      </c>
+      <c r="G39">
+        <v>4826.63</v>
+      </c>
+      <c r="H39">
+        <v>4794.8500000000004</v>
+      </c>
+      <c r="I39">
+        <v>4846.62</v>
+      </c>
+      <c r="J39">
+        <v>4898.79</v>
+      </c>
+      <c r="K39">
+        <v>4868.22</v>
+      </c>
+      <c r="L39">
+        <v>4936.43</v>
+      </c>
+      <c r="M39">
+        <v>4892.99</v>
+      </c>
+      <c r="N39">
+        <v>4919.38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>4829.46</v>
+      </c>
+      <c r="D40">
+        <v>4835.8900000000003</v>
+      </c>
+      <c r="E40">
+        <v>4818.1099999999997</v>
+      </c>
+      <c r="F40">
+        <v>4556.8100000000004</v>
+      </c>
+      <c r="G40">
+        <v>4876.92</v>
+      </c>
+      <c r="H40">
+        <v>4886.37</v>
+      </c>
+      <c r="I40">
+        <v>4871.12</v>
+      </c>
+      <c r="J40">
+        <v>4946.8599999999997</v>
+      </c>
+      <c r="K40">
+        <v>4890.0200000000004</v>
+      </c>
+      <c r="L40">
+        <v>4907.59</v>
+      </c>
+      <c r="M40">
+        <v>4926.78</v>
+      </c>
+      <c r="N40">
+        <v>4925.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>4820.95</v>
+      </c>
+      <c r="D41">
+        <v>4522.22</v>
+      </c>
+      <c r="E41">
+        <v>4456.41</v>
+      </c>
+      <c r="F41">
+        <v>4542.91</v>
+      </c>
+      <c r="G41">
+        <v>4558.71</v>
+      </c>
+      <c r="H41">
+        <v>4586.79</v>
+      </c>
+      <c r="I41">
+        <v>4843.75</v>
+      </c>
+      <c r="J41">
+        <v>4815.99</v>
+      </c>
+      <c r="K41">
+        <v>4939.3999999999996</v>
+      </c>
+      <c r="L41">
+        <v>4937.91</v>
+      </c>
+      <c r="M41">
+        <v>4481.3999999999996</v>
+      </c>
+      <c r="N41">
+        <v>4890.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>4500.4799999999996</v>
+      </c>
+      <c r="D42">
+        <v>4525.34</v>
+      </c>
+      <c r="E42">
+        <v>4766.25</v>
+      </c>
+      <c r="F42">
+        <v>4848.05</v>
+      </c>
+      <c r="G42">
+        <v>4836.6099999999997</v>
+      </c>
+      <c r="H42">
+        <v>4579.01</v>
+      </c>
+      <c r="I42">
+        <v>4877.6899999999996</v>
+      </c>
+      <c r="J42">
+        <v>5008.87</v>
+      </c>
+      <c r="K42">
+        <v>4958.84</v>
+      </c>
+      <c r="L42">
+        <v>4888.5600000000004</v>
+      </c>
+      <c r="M42">
+        <v>4938.66</v>
+      </c>
+      <c r="N42">
+        <v>4910.53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>4851.6899999999996</v>
+      </c>
+      <c r="D43">
+        <v>4512.88</v>
+      </c>
+      <c r="E43">
+        <v>4552.38</v>
+      </c>
+      <c r="F43">
+        <v>4893.67</v>
+      </c>
+      <c r="G43">
+        <v>4529.09</v>
+      </c>
+      <c r="H43">
+        <v>4864.6099999999997</v>
+      </c>
+      <c r="I43">
+        <v>4961.09</v>
+      </c>
+      <c r="J43">
+        <v>4894.3999999999996</v>
+      </c>
+      <c r="K43">
+        <v>4937.17</v>
+      </c>
+      <c r="L43">
+        <v>4941.04</v>
+      </c>
+      <c r="M43">
+        <v>4898.0600000000004</v>
+      </c>
+      <c r="N43">
+        <v>4842.32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>4856.68</v>
+      </c>
+      <c r="D44">
+        <v>4857.3999999999996</v>
+      </c>
+      <c r="E44">
+        <v>4491.2299999999996</v>
+      </c>
+      <c r="F44">
+        <v>4760.0200000000004</v>
+      </c>
+      <c r="G44">
+        <v>4907.59</v>
+      </c>
+      <c r="H44">
+        <v>4821.66</v>
+      </c>
+      <c r="I44">
+        <v>4879.82</v>
+      </c>
+      <c r="J44">
+        <v>4920.12</v>
+      </c>
+      <c r="K44">
+        <v>4974.6499999999996</v>
+      </c>
+      <c r="L44">
+        <v>4932.51</v>
+      </c>
+      <c r="M44">
+        <v>4937.91</v>
+      </c>
+      <c r="N44">
+        <v>4953.59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>4748.3</v>
+      </c>
+      <c r="D45">
+        <v>4789.24</v>
+      </c>
+      <c r="E45">
+        <v>4774.59</v>
+      </c>
+      <c r="F45">
+        <v>4751.05</v>
+      </c>
+      <c r="G45">
+        <v>4553.6400000000003</v>
+      </c>
+      <c r="H45">
+        <v>4863.16</v>
+      </c>
+      <c r="I45">
+        <v>4869.67</v>
+      </c>
+      <c r="J45">
+        <v>4890.75</v>
+      </c>
+      <c r="K45">
+        <v>4882</v>
+      </c>
+      <c r="L45">
+        <v>4854.5200000000004</v>
+      </c>
+      <c r="M45">
+        <v>4917.17</v>
+      </c>
+      <c r="N45">
+        <v>4963.34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>4815.99</v>
+      </c>
+      <c r="D46">
+        <v>4878.37</v>
+      </c>
+      <c r="E46">
+        <v>4869</v>
+      </c>
+      <c r="F46">
+        <v>4796.26</v>
+      </c>
+      <c r="G46">
+        <v>4826.63</v>
+      </c>
+      <c r="H46">
+        <v>4830.1899999999996</v>
+      </c>
+      <c r="I46">
+        <v>4883.46</v>
+      </c>
+      <c r="J46">
+        <v>4872.57</v>
+      </c>
+      <c r="K46">
+        <v>4968.6099999999997</v>
+      </c>
+      <c r="L46">
+        <v>4853.08</v>
+      </c>
+      <c r="M46">
+        <v>4935.68</v>
+      </c>
+      <c r="N46">
+        <v>4940.1499999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>4806.1000000000004</v>
+      </c>
+      <c r="D47">
+        <v>4506.67</v>
+      </c>
+      <c r="E47">
+        <v>4584.22</v>
+      </c>
+      <c r="F47">
+        <v>4807.51</v>
+      </c>
+      <c r="G47">
+        <v>4830.8999999999996</v>
+      </c>
+      <c r="H47">
+        <v>4785.75</v>
+      </c>
+      <c r="I47">
+        <v>4955.09</v>
+      </c>
+      <c r="J47">
+        <v>4720.25</v>
+      </c>
+      <c r="K47">
+        <v>4891.4799999999996</v>
+      </c>
+      <c r="L47">
+        <v>4861.72</v>
+      </c>
+      <c r="M47">
+        <v>4942.38</v>
+      </c>
+      <c r="N47">
+        <v>4924.5600000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <f>ROUND(AVERAGE(C38:C47),2)</f>
+        <v>4739.38</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49:N49" si="9">ROUND(AVERAGE(D38:D47),2)</f>
+        <v>4681.3999999999996</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="9"/>
+        <v>4668.13</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="9"/>
+        <v>4732.7</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="9"/>
+        <v>4761.49</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="9"/>
+        <v>4782.84</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="9"/>
+        <v>4886.67</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="9"/>
+        <v>4851.3999999999996</v>
+      </c>
+      <c r="K49" s="3">
+        <f t="shared" si="9"/>
+        <v>4920.26</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="9"/>
+        <v>4907.82</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="9"/>
+        <v>4883.0600000000004</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="9"/>
+        <v>4919.6000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <f>MAX(C38:C47)</f>
+        <v>4856.68</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ref="D50:N50" si="10">MAX(D38:D47)</f>
+        <v>4878.37</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="10"/>
+        <v>4869</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="10"/>
+        <v>4893.67</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="10"/>
+        <v>4907.59</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="10"/>
+        <v>4886.37</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="10"/>
+        <v>4961.09</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="10"/>
+        <v>5008.87</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="10"/>
+        <v>4974.6499999999996</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="10"/>
+        <v>4964.8500000000004</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="10"/>
+        <v>4959.59</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="10"/>
+        <v>4963.34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <f>MIN(C38:C47)</f>
+        <v>4500.4799999999996</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:N51" si="11">MIN(D38:D47)</f>
+        <v>4506.67</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="11"/>
+        <v>4456.41</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="11"/>
+        <v>4542.91</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="11"/>
+        <v>4529.09</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="11"/>
+        <v>4579.01</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="11"/>
+        <v>4843.75</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="11"/>
+        <v>4545.43</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="11"/>
+        <v>4868.22</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="11"/>
+        <v>4853.08</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="11"/>
+        <v>4481.3999999999996</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="11"/>
+        <v>4842.32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <f>ROUND(STDEV(C38:C47),2)</f>
+        <v>134.16999999999999</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" ref="D52:N52" si="12">ROUND(STDEV(D38:D47),2)</f>
+        <v>170.84</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="12"/>
+        <v>157.09</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="12"/>
+        <v>127.08</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="12"/>
+        <v>150.31</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="12"/>
+        <v>109.97</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="12"/>
+        <v>131.99</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="12"/>
+        <v>39.630000000000003</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="12"/>
+        <v>40.86</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="12"/>
+        <v>142.58000000000001</v>
+      </c>
+      <c r="N52" s="4">
+        <f t="shared" si="12"/>
+        <v>34.119999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>